<commit_message>
added clean data rules to makefile
</commit_message>
<xml_diff>
--- a/f75_dataset/f75_codebook.xlsx
+++ b/f75_dataset/f75_codebook.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emilywu/Library/CloudStorage/OneDrive-EmoryUniversity/Core/Year 3/DATA 550/Midterm project data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nazizanaeer/Documents/R/DATA550/midterm/f75_dataset/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{33F33758-0306-2048-8E8B-E081D3876C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40290569-30B6-794E-BA16-0DBF0FABB86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6640" yWindow="2200" windowWidth="28040" windowHeight="17440" xr2:uid="{5909F88D-4FDC-9546-83D5-F29C41269541}"/>
+    <workbookView xWindow="1360" yWindow="740" windowWidth="28040" windowHeight="17300" xr2:uid="{5909F88D-4FDC-9546-83D5-F29C41269541}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -312,7 +312,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -322,6 +322,12 @@
     </font>
     <font>
       <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -409,7 +415,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -422,6 +428,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,8 +780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3C5895-921C-A04C-AC44-E73F09B77FE8}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" zoomScale="116" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -978,10 +987,10 @@
       <c r="C20" s="3"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
+      <c r="A21" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="12" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="3"/>
@@ -1059,10 +1068,10 @@
       <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="B30" s="11" t="s">
         <v>48</v>
       </c>
       <c r="C30" s="5"/>
@@ -1104,10 +1113,10 @@
       <c r="C34" s="6"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="10" t="s">
         <v>79</v>
       </c>
       <c r="C35" s="7"/>
@@ -1158,10 +1167,10 @@
       <c r="C40" s="7"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="7" t="s">
+      <c r="A41" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B41" s="7" t="s">
+      <c r="B41" s="10" t="s">
         <v>77</v>
       </c>
       <c r="C41" s="7"/>

</xml_diff>